<commit_message>
Diagnostic Report IG - first draft of Observation (Atomic Other Diagnostic Observation)
</commit_message>
<xml_diff>
--- a/output/EventSummary/patient-mhr-1.xlsx
+++ b/output/EventSummary/patient-mhr-1.xlsx
@@ -6918,7 +6918,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F43" t="s" s="2">
         <v>51</v>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F47" t="s" s="2">
         <v>51</v>

</xml_diff>